<commit_message>
uploaded the files from a while
</commit_message>
<xml_diff>
--- a/files/Matières/EPS/T1/temps fille et gaçon convertis.xlsx
+++ b/files/Matières/EPS/T1/temps fille et gaçon convertis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry PC\Documents\001 Github prog Sharing\Backup-of-matiere\files\Matières\EPS\T1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D5A58EB-C89B-4D4D-B016-9F62CAF274B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3A6A49-F4BC-43FF-956F-6372EDDC1F4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{A7CA7E09-31A3-4572-9AB2-7E0D1B85D51B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="72">
   <si>
     <t>9'03</t>
   </si>
@@ -187,13 +187,76 @@
   </si>
   <si>
     <t>temps</t>
+  </si>
+  <si>
+    <t>9'25</t>
+  </si>
+  <si>
+    <t>9'47</t>
+  </si>
+  <si>
+    <t>10'09</t>
+  </si>
+  <si>
+    <t>10'31</t>
+  </si>
+  <si>
+    <t>10'53</t>
+  </si>
+  <si>
+    <t>11'15</t>
+  </si>
+  <si>
+    <t>11'37</t>
+  </si>
+  <si>
+    <t>Mins</t>
+  </si>
+  <si>
+    <t>Secs</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>All in secs</t>
+  </si>
+  <si>
+    <t>Incrémentation avec pas</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
+  <si>
+    <t>secs</t>
+  </si>
+  <si>
+    <t>7'47</t>
+  </si>
+  <si>
+    <t>8'25</t>
+  </si>
+  <si>
+    <t>8'06</t>
+  </si>
+  <si>
+    <t>8'44</t>
+  </si>
+  <si>
+    <t>9'22</t>
+  </si>
+  <si>
+    <t>9'41</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,16 +271,83 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -255,11 +385,321 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -268,11 +708,75 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2612,10 +3116,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C427C7C-1CEF-4716-A5C5-0BEFAA7EA713}">
-  <dimension ref="B1:R23"/>
+  <dimension ref="B1:R57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N6" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3:R22"/>
+    <sheetView tabSelected="1" topLeftCell="D40" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2624,12 +3128,12 @@
       <c r="D1" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="4"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
@@ -2659,10 +3163,10 @@
       <c r="L2" t="s">
         <v>42</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="4" t="s">
         <v>47</v>
       </c>
       <c r="O2" t="s">
@@ -2693,7 +3197,7 @@
         <v>543</v>
       </c>
       <c r="H3" s="1">
-        <f>D3*60+E3</f>
+        <f t="shared" ref="H3:H22" si="0">D3*60+E3</f>
         <v>543</v>
       </c>
       <c r="I3" s="2">
@@ -2716,7 +3220,7 @@
         <v>448</v>
       </c>
       <c r="Q3" s="1">
-        <f>M3*60+N3</f>
+        <f t="shared" ref="Q3:Q22" si="1">M3*60+N3</f>
         <v>448</v>
       </c>
       <c r="R3" s="2">
@@ -2741,7 +3245,7 @@
         <v>521</v>
       </c>
       <c r="H4" s="1">
-        <f>D4*60+E4</f>
+        <f t="shared" si="0"/>
         <v>521</v>
       </c>
       <c r="I4" s="2">
@@ -2764,7 +3268,7 @@
         <v>429</v>
       </c>
       <c r="Q4" s="1">
-        <f>M4*60+N4</f>
+        <f t="shared" si="1"/>
         <v>429</v>
       </c>
       <c r="R4" s="2">
@@ -2785,7 +3289,7 @@
         <v>20</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" ref="F5:F23" si="0">D5*60+E5</f>
+        <f t="shared" ref="F5:F22" si="2">D5*60+E5</f>
         <v>500</v>
       </c>
       <c r="H5" s="1">
@@ -2808,11 +3312,11 @@
         <v>51</v>
       </c>
       <c r="O5" s="1">
-        <f t="shared" ref="O5:O22" si="1">M5*60+N5</f>
+        <f t="shared" ref="O5:O22" si="3">M5*60+N5</f>
         <v>411</v>
       </c>
       <c r="Q5" s="1">
-        <f>M5*60+N5</f>
+        <f t="shared" si="1"/>
         <v>411</v>
       </c>
       <c r="R5" s="2">
@@ -2833,13 +3337,13 @@
         <v>0</v>
       </c>
       <c r="F6" s="1">
+        <f t="shared" si="2"/>
+        <v>480</v>
+      </c>
+      <c r="H6" s="1">
         <f t="shared" si="0"/>
         <v>480</v>
       </c>
-      <c r="H6" s="1">
-        <f>D6*60+E6</f>
-        <v>480</v>
-      </c>
       <c r="I6" s="2">
         <v>2.8</v>
       </c>
@@ -2856,11 +3360,11 @@
         <v>34</v>
       </c>
       <c r="O6" s="1">
+        <f t="shared" si="3"/>
+        <v>394</v>
+      </c>
+      <c r="Q6" s="1">
         <f t="shared" si="1"/>
-        <v>394</v>
-      </c>
-      <c r="Q6" s="1">
-        <f>M6*60+N6</f>
         <v>394</v>
       </c>
       <c r="R6" s="2">
@@ -2881,13 +3385,13 @@
         <v>41</v>
       </c>
       <c r="F7" s="1">
+        <f t="shared" si="2"/>
+        <v>461</v>
+      </c>
+      <c r="H7" s="1">
         <f t="shared" si="0"/>
         <v>461</v>
       </c>
-      <c r="H7" s="1">
-        <f>D7*60+E7</f>
-        <v>461</v>
-      </c>
       <c r="I7" s="2">
         <v>3.5</v>
       </c>
@@ -2904,11 +3408,11 @@
         <v>19</v>
       </c>
       <c r="O7" s="1">
+        <f t="shared" si="3"/>
+        <v>379</v>
+      </c>
+      <c r="Q7" s="1">
         <f t="shared" si="1"/>
-        <v>379</v>
-      </c>
-      <c r="Q7" s="1">
-        <f>M7*60+N7</f>
         <v>379</v>
       </c>
       <c r="R7" s="2">
@@ -2929,13 +3433,13 @@
         <v>24</v>
       </c>
       <c r="F8" s="1">
+        <f t="shared" si="2"/>
+        <v>444</v>
+      </c>
+      <c r="H8" s="1">
         <f t="shared" si="0"/>
         <v>444</v>
       </c>
-      <c r="H8" s="1">
-        <f>D8*60+E8</f>
-        <v>444</v>
-      </c>
       <c r="I8" s="2">
         <v>4.2</v>
       </c>
@@ -2952,11 +3456,11 @@
         <v>5</v>
       </c>
       <c r="O8" s="1">
+        <f t="shared" si="3"/>
+        <v>365</v>
+      </c>
+      <c r="Q8" s="1">
         <f t="shared" si="1"/>
-        <v>365</v>
-      </c>
-      <c r="Q8" s="1">
-        <f>M8*60+N8</f>
         <v>365</v>
       </c>
       <c r="R8" s="2">
@@ -2977,13 +3481,13 @@
         <v>8</v>
       </c>
       <c r="F9" s="1">
+        <f t="shared" si="2"/>
+        <v>428</v>
+      </c>
+      <c r="H9" s="1">
         <f t="shared" si="0"/>
         <v>428</v>
       </c>
-      <c r="H9" s="1">
-        <f>D9*60+E9</f>
-        <v>428</v>
-      </c>
       <c r="I9" s="2">
         <v>4.9000000000000004</v>
       </c>
@@ -3000,11 +3504,11 @@
         <v>52</v>
       </c>
       <c r="O9" s="1">
+        <f t="shared" si="3"/>
+        <v>352</v>
+      </c>
+      <c r="Q9" s="1">
         <f t="shared" si="1"/>
-        <v>352</v>
-      </c>
-      <c r="Q9" s="1">
-        <f>M9*60+N9</f>
         <v>352</v>
       </c>
       <c r="R9" s="2">
@@ -3025,13 +3529,13 @@
         <v>53</v>
       </c>
       <c r="F10" s="1">
+        <f t="shared" si="2"/>
+        <v>413</v>
+      </c>
+      <c r="H10" s="1">
         <f t="shared" si="0"/>
         <v>413</v>
       </c>
-      <c r="H10" s="1">
-        <f>D10*60+E10</f>
-        <v>413</v>
-      </c>
       <c r="I10" s="2">
         <v>5.6</v>
       </c>
@@ -3048,11 +3552,11 @@
         <v>40</v>
       </c>
       <c r="O10" s="1">
+        <f t="shared" si="3"/>
+        <v>340</v>
+      </c>
+      <c r="Q10" s="1">
         <f t="shared" si="1"/>
-        <v>340</v>
-      </c>
-      <c r="Q10" s="1">
-        <f>M10*60+N10</f>
         <v>340</v>
       </c>
       <c r="R10" s="2">
@@ -3073,13 +3577,13 @@
         <v>39</v>
       </c>
       <c r="F11" s="1">
+        <f t="shared" si="2"/>
+        <v>399</v>
+      </c>
+      <c r="H11" s="1">
         <f t="shared" si="0"/>
         <v>399</v>
       </c>
-      <c r="H11" s="1">
-        <f>D11*60+E11</f>
-        <v>399</v>
-      </c>
       <c r="I11" s="2">
         <v>6.3</v>
       </c>
@@ -3096,11 +3600,11 @@
         <v>29</v>
       </c>
       <c r="O11" s="1">
+        <f t="shared" si="3"/>
+        <v>329</v>
+      </c>
+      <c r="Q11" s="1">
         <f t="shared" si="1"/>
-        <v>329</v>
-      </c>
-      <c r="Q11" s="1">
-        <f>M11*60+N11</f>
         <v>329</v>
       </c>
       <c r="R11" s="2">
@@ -3121,13 +3625,13 @@
         <v>26</v>
       </c>
       <c r="F12" s="1">
+        <f t="shared" si="2"/>
+        <v>386</v>
+      </c>
+      <c r="H12" s="1">
         <f t="shared" si="0"/>
         <v>386</v>
       </c>
-      <c r="H12" s="1">
-        <f>D12*60+E12</f>
-        <v>386</v>
-      </c>
       <c r="I12" s="3">
         <v>7</v>
       </c>
@@ -3144,11 +3648,11 @@
         <v>19</v>
       </c>
       <c r="O12" s="1">
+        <f t="shared" si="3"/>
+        <v>319</v>
+      </c>
+      <c r="Q12" s="1">
         <f t="shared" si="1"/>
-        <v>319</v>
-      </c>
-      <c r="Q12" s="1">
-        <f>M12*60+N12</f>
         <v>319</v>
       </c>
       <c r="R12" s="3">
@@ -3169,13 +3673,13 @@
         <v>20</v>
       </c>
       <c r="F13" s="1">
+        <f t="shared" si="2"/>
+        <v>380</v>
+      </c>
+      <c r="H13" s="1">
         <f t="shared" si="0"/>
         <v>380</v>
       </c>
-      <c r="H13" s="1">
-        <f>D13*60+E13</f>
-        <v>380</v>
-      </c>
       <c r="I13" s="3">
         <v>7.7</v>
       </c>
@@ -3192,11 +3696,11 @@
         <v>11</v>
       </c>
       <c r="O13" s="1">
+        <f t="shared" si="3"/>
+        <v>311</v>
+      </c>
+      <c r="Q13" s="1">
         <f t="shared" si="1"/>
-        <v>311</v>
-      </c>
-      <c r="Q13" s="1">
-        <f>M13*60+N13</f>
         <v>311</v>
       </c>
       <c r="R13" s="3">
@@ -3217,13 +3721,13 @@
         <v>13</v>
       </c>
       <c r="F14" s="1">
+        <f t="shared" si="2"/>
+        <v>373</v>
+      </c>
+      <c r="H14" s="1">
         <f t="shared" si="0"/>
         <v>373</v>
       </c>
-      <c r="H14" s="1">
-        <f>D14*60+E14</f>
-        <v>373</v>
-      </c>
       <c r="I14" s="3">
         <v>8.4</v>
       </c>
@@ -3240,11 +3744,11 @@
         <v>3</v>
       </c>
       <c r="O14" s="1">
+        <f t="shared" si="3"/>
+        <v>303</v>
+      </c>
+      <c r="Q14" s="1">
         <f t="shared" si="1"/>
-        <v>303</v>
-      </c>
-      <c r="Q14" s="1">
-        <f>M14*60+N14</f>
         <v>303</v>
       </c>
       <c r="R14" s="3">
@@ -3265,13 +3769,13 @@
         <v>7</v>
       </c>
       <c r="F15" s="1">
+        <f t="shared" si="2"/>
+        <v>367</v>
+      </c>
+      <c r="H15" s="1">
         <f t="shared" si="0"/>
         <v>367</v>
       </c>
-      <c r="H15" s="1">
-        <f>D15*60+E15</f>
-        <v>367</v>
-      </c>
       <c r="I15" s="3">
         <v>9.1</v>
       </c>
@@ -3288,11 +3792,11 @@
         <v>55</v>
       </c>
       <c r="O15" s="1">
+        <f t="shared" si="3"/>
+        <v>295</v>
+      </c>
+      <c r="Q15" s="1">
         <f t="shared" si="1"/>
-        <v>295</v>
-      </c>
-      <c r="Q15" s="1">
-        <f>M15*60+N15</f>
         <v>295</v>
       </c>
       <c r="R15" s="3">
@@ -3313,13 +3817,13 @@
         <v>1</v>
       </c>
       <c r="F16" s="1">
+        <f t="shared" si="2"/>
+        <v>361</v>
+      </c>
+      <c r="H16" s="1">
         <f t="shared" si="0"/>
         <v>361</v>
       </c>
-      <c r="H16" s="1">
-        <f>D16*60+E16</f>
-        <v>361</v>
-      </c>
       <c r="I16" s="3">
         <v>9.8000000000000007</v>
       </c>
@@ -3336,11 +3840,11 @@
         <v>51</v>
       </c>
       <c r="O16" s="1">
+        <f t="shared" si="3"/>
+        <v>291</v>
+      </c>
+      <c r="Q16" s="1">
         <f t="shared" si="1"/>
-        <v>291</v>
-      </c>
-      <c r="Q16" s="1">
-        <f>M16*60+N16</f>
         <v>291</v>
       </c>
       <c r="R16" s="3">
@@ -3361,13 +3865,13 @@
         <v>55</v>
       </c>
       <c r="F17" s="1">
+        <f t="shared" si="2"/>
+        <v>355</v>
+      </c>
+      <c r="H17" s="1">
         <f t="shared" si="0"/>
         <v>355</v>
       </c>
-      <c r="H17" s="1">
-        <f>D17*60+E17</f>
-        <v>355</v>
-      </c>
       <c r="I17" s="3">
         <v>10.5</v>
       </c>
@@ -3384,11 +3888,11 @@
         <v>47</v>
       </c>
       <c r="O17" s="1">
+        <f t="shared" si="3"/>
+        <v>287</v>
+      </c>
+      <c r="Q17" s="1">
         <f t="shared" si="1"/>
-        <v>287</v>
-      </c>
-      <c r="Q17" s="1">
-        <f>M17*60+N17</f>
         <v>287</v>
       </c>
       <c r="R17" s="3">
@@ -3409,13 +3913,13 @@
         <v>49</v>
       </c>
       <c r="F18" s="1">
+        <f t="shared" si="2"/>
+        <v>349</v>
+      </c>
+      <c r="H18" s="1">
         <f t="shared" si="0"/>
         <v>349</v>
       </c>
-      <c r="H18" s="1">
-        <f>D18*60+E18</f>
-        <v>349</v>
-      </c>
       <c r="I18" s="3">
         <v>11.2</v>
       </c>
@@ -3432,11 +3936,11 @@
         <v>43</v>
       </c>
       <c r="O18" s="1">
+        <f t="shared" si="3"/>
+        <v>283</v>
+      </c>
+      <c r="Q18" s="1">
         <f t="shared" si="1"/>
-        <v>283</v>
-      </c>
-      <c r="Q18" s="1">
-        <f>M18*60+N18</f>
         <v>283</v>
       </c>
       <c r="R18" s="3">
@@ -3457,13 +3961,13 @@
         <v>43</v>
       </c>
       <c r="F19" s="1">
+        <f t="shared" si="2"/>
+        <v>343</v>
+      </c>
+      <c r="H19" s="1">
         <f t="shared" si="0"/>
         <v>343</v>
       </c>
-      <c r="H19" s="1">
-        <f>D19*60+E19</f>
-        <v>343</v>
-      </c>
       <c r="I19" s="3">
         <v>11.9</v>
       </c>
@@ -3480,11 +3984,11 @@
         <v>40</v>
       </c>
       <c r="O19" s="1">
+        <f t="shared" si="3"/>
+        <v>280</v>
+      </c>
+      <c r="Q19" s="1">
         <f t="shared" si="1"/>
-        <v>280</v>
-      </c>
-      <c r="Q19" s="1">
-        <f>M19*60+N19</f>
         <v>280</v>
       </c>
       <c r="R19" s="3">
@@ -3505,13 +4009,13 @@
         <v>37</v>
       </c>
       <c r="F20" s="1">
+        <f t="shared" si="2"/>
+        <v>337</v>
+      </c>
+      <c r="H20" s="1">
         <f t="shared" si="0"/>
         <v>337</v>
       </c>
-      <c r="H20" s="1">
-        <f>D20*60+E20</f>
-        <v>337</v>
-      </c>
       <c r="I20" s="3">
         <v>12.6</v>
       </c>
@@ -3528,11 +4032,11 @@
         <v>37</v>
       </c>
       <c r="O20" s="1">
+        <f t="shared" si="3"/>
+        <v>277</v>
+      </c>
+      <c r="Q20" s="1">
         <f t="shared" si="1"/>
-        <v>277</v>
-      </c>
-      <c r="Q20" s="1">
-        <f>M20*60+N20</f>
         <v>277</v>
       </c>
       <c r="R20" s="3">
@@ -3553,13 +4057,13 @@
         <v>31</v>
       </c>
       <c r="F21" s="1">
+        <f t="shared" si="2"/>
+        <v>331</v>
+      </c>
+      <c r="H21" s="1">
         <f t="shared" si="0"/>
         <v>331</v>
       </c>
-      <c r="H21" s="1">
-        <f>D21*60+E21</f>
-        <v>331</v>
-      </c>
       <c r="I21" s="3">
         <v>13.3</v>
       </c>
@@ -3576,11 +4080,11 @@
         <v>34</v>
       </c>
       <c r="O21" s="1">
+        <f t="shared" si="3"/>
+        <v>274</v>
+      </c>
+      <c r="Q21" s="1">
         <f t="shared" si="1"/>
-        <v>274</v>
-      </c>
-      <c r="Q21" s="1">
-        <f>M21*60+N21</f>
         <v>274</v>
       </c>
       <c r="R21" s="3">
@@ -3601,13 +4105,13 @@
         <v>25</v>
       </c>
       <c r="F22" s="1">
+        <f t="shared" si="2"/>
+        <v>325</v>
+      </c>
+      <c r="H22" s="1">
         <f t="shared" si="0"/>
         <v>325</v>
       </c>
-      <c r="H22" s="1">
-        <f>D22*60+E22</f>
-        <v>325</v>
-      </c>
       <c r="I22" s="3">
         <v>14</v>
       </c>
@@ -3624,11 +4128,11 @@
         <v>31</v>
       </c>
       <c r="O22" s="1">
+        <f t="shared" si="3"/>
+        <v>271</v>
+      </c>
+      <c r="Q22" s="1">
         <f t="shared" si="1"/>
-        <v>271</v>
-      </c>
-      <c r="Q22" s="1">
-        <f>M22*60+N22</f>
         <v>271</v>
       </c>
       <c r="R22" s="3">
@@ -3638,11 +4142,598 @@
     <row r="23" spans="2:18" x14ac:dyDescent="0.45">
       <c r="F23" s="1"/>
     </row>
+    <row r="39" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="40" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B40" s="56"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="56"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="12"/>
+      <c r="M40" s="12"/>
+      <c r="N40" s="12"/>
+      <c r="O40" s="12"/>
+      <c r="P40" s="12"/>
+      <c r="Q40" s="12"/>
+      <c r="R40" s="56"/>
+    </row>
+    <row r="41" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B41" s="36"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="47"/>
+      <c r="E41" s="47"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="H41" s="38">
+        <v>15</v>
+      </c>
+      <c r="J41" s="36"/>
+      <c r="K41" s="55"/>
+      <c r="N41" s="54"/>
+      <c r="O41" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="P41" s="39">
+        <v>22</v>
+      </c>
+      <c r="R41" s="36"/>
+    </row>
+    <row r="42" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B42" s="36"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="H42" s="24">
+        <v>22</v>
+      </c>
+      <c r="J42" s="36"/>
+      <c r="L42" s="46"/>
+      <c r="M42" s="48"/>
+      <c r="O42" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="P42" s="10">
+        <v>19</v>
+      </c>
+      <c r="R42" s="36"/>
+    </row>
+    <row r="43" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B43" s="36"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="53"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="25"/>
+      <c r="J43" s="36"/>
+      <c r="L43" s="51"/>
+      <c r="M43" s="53"/>
+      <c r="O43" s="28"/>
+      <c r="P43" s="7"/>
+      <c r="R43" s="36"/>
+    </row>
+    <row r="44" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B44" s="36"/>
+      <c r="C44" s="58"/>
+      <c r="D44" s="52"/>
+      <c r="E44" s="52"/>
+      <c r="F44" s="59"/>
+      <c r="G44" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="H44" s="26">
+        <f>H41+H42</f>
+        <v>37</v>
+      </c>
+      <c r="J44" s="36"/>
+      <c r="K44" s="54"/>
+      <c r="N44" s="54"/>
+      <c r="O44" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="P44" s="8">
+        <f>P41+P42</f>
+        <v>41</v>
+      </c>
+      <c r="R44" s="36"/>
+    </row>
+    <row r="45" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B45" s="36"/>
+      <c r="C45" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F45" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G45" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="H45" s="23"/>
+      <c r="I45" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="J45" s="36"/>
+      <c r="K45" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="L45" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="M45" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="N45" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="O45" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="P45" s="20"/>
+      <c r="Q45" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="R45" s="36"/>
+    </row>
+    <row r="46" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B46" s="36"/>
+      <c r="C46" s="34">
+        <v>0.7</v>
+      </c>
+      <c r="D46" s="11">
+        <v>9</v>
+      </c>
+      <c r="E46" s="15">
+        <v>3</v>
+      </c>
+      <c r="F46" s="18">
+        <f>D46*60+E46</f>
+        <v>543</v>
+      </c>
+      <c r="G46" s="21">
+        <f>F46+H42</f>
+        <v>565</v>
+      </c>
+      <c r="H46" s="21"/>
+      <c r="I46" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="J46" s="36"/>
+      <c r="K46" s="34">
+        <v>0.7</v>
+      </c>
+      <c r="L46" s="11">
+        <v>7</v>
+      </c>
+      <c r="M46" s="15">
+        <v>28</v>
+      </c>
+      <c r="N46" s="18">
+        <f>L46*60+M46</f>
+        <v>448</v>
+      </c>
+      <c r="O46" s="21">
+        <f>N46+P42</f>
+        <v>467</v>
+      </c>
+      <c r="P46" s="21"/>
+      <c r="Q46" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="R46" s="36"/>
+    </row>
+    <row r="47" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B47" s="36"/>
+      <c r="C47" s="35">
+        <f>C46-0.1</f>
+        <v>0.6</v>
+      </c>
+      <c r="D47" s="9">
+        <v>9</v>
+      </c>
+      <c r="E47" s="16">
+        <v>25</v>
+      </c>
+      <c r="F47" s="19">
+        <f t="shared" ref="F47:F53" si="4">D47*60+E47</f>
+        <v>565</v>
+      </c>
+      <c r="G47" s="22">
+        <f>F47+H42</f>
+        <v>587</v>
+      </c>
+      <c r="H47" s="22"/>
+      <c r="I47" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="J47" s="36"/>
+      <c r="K47" s="35">
+        <f>K46-0.1</f>
+        <v>0.6</v>
+      </c>
+      <c r="L47" s="9">
+        <v>7</v>
+      </c>
+      <c r="M47" s="16">
+        <v>47</v>
+      </c>
+      <c r="N47" s="19">
+        <f t="shared" ref="N47:N53" si="5">L47*60+M47</f>
+        <v>467</v>
+      </c>
+      <c r="O47" s="22">
+        <f>N47+P42</f>
+        <v>486</v>
+      </c>
+      <c r="P47" s="22"/>
+      <c r="Q47" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="R47" s="36"/>
+    </row>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B48" s="36"/>
+      <c r="C48" s="35">
+        <f t="shared" ref="C48:C53" si="6">C47-0.1</f>
+        <v>0.5</v>
+      </c>
+      <c r="D48" s="9">
+        <v>9</v>
+      </c>
+      <c r="E48" s="16">
+        <v>47</v>
+      </c>
+      <c r="F48" s="19">
+        <f t="shared" si="4"/>
+        <v>587</v>
+      </c>
+      <c r="G48" s="22">
+        <f>F48+H42</f>
+        <v>609</v>
+      </c>
+      <c r="H48" s="22"/>
+      <c r="I48" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="J48" s="36"/>
+      <c r="K48" s="35">
+        <f t="shared" ref="K48:K57" si="7">K47-0.1</f>
+        <v>0.5</v>
+      </c>
+      <c r="L48" s="9">
+        <v>8</v>
+      </c>
+      <c r="M48" s="16">
+        <v>6</v>
+      </c>
+      <c r="N48" s="19">
+        <f t="shared" si="5"/>
+        <v>486</v>
+      </c>
+      <c r="O48" s="22">
+        <f>N48+P42</f>
+        <v>505</v>
+      </c>
+      <c r="P48" s="22"/>
+      <c r="Q48" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="R48" s="36"/>
+    </row>
+    <row r="49" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B49" s="36"/>
+      <c r="C49" s="35">
+        <f t="shared" si="6"/>
+        <v>0.4</v>
+      </c>
+      <c r="D49" s="9">
+        <v>10</v>
+      </c>
+      <c r="E49" s="16">
+        <v>9</v>
+      </c>
+      <c r="F49" s="19">
+        <f t="shared" si="4"/>
+        <v>609</v>
+      </c>
+      <c r="G49" s="22">
+        <f>F49+H42</f>
+        <v>631</v>
+      </c>
+      <c r="H49" s="22"/>
+      <c r="I49" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="J49" s="36"/>
+      <c r="K49" s="35">
+        <f t="shared" si="7"/>
+        <v>0.4</v>
+      </c>
+      <c r="L49" s="9">
+        <v>8</v>
+      </c>
+      <c r="M49" s="16">
+        <v>25</v>
+      </c>
+      <c r="N49" s="19">
+        <f t="shared" si="5"/>
+        <v>505</v>
+      </c>
+      <c r="O49" s="22">
+        <f>N49+P42</f>
+        <v>524</v>
+      </c>
+      <c r="P49" s="22"/>
+      <c r="Q49" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="R49" s="36"/>
+    </row>
+    <row r="50" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B50" s="36"/>
+      <c r="C50" s="35">
+        <f t="shared" si="6"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="D50" s="9">
+        <v>10</v>
+      </c>
+      <c r="E50" s="16">
+        <v>31</v>
+      </c>
+      <c r="F50" s="19">
+        <f t="shared" si="4"/>
+        <v>631</v>
+      </c>
+      <c r="G50" s="22">
+        <f>F50+H42</f>
+        <v>653</v>
+      </c>
+      <c r="H50" s="22"/>
+      <c r="I50" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="J50" s="36"/>
+      <c r="K50" s="35">
+        <f t="shared" si="7"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="L50" s="9">
+        <v>8</v>
+      </c>
+      <c r="M50" s="16">
+        <v>44</v>
+      </c>
+      <c r="N50" s="19">
+        <f t="shared" si="5"/>
+        <v>524</v>
+      </c>
+      <c r="O50" s="22">
+        <f>N50+P42</f>
+        <v>543</v>
+      </c>
+      <c r="P50" s="22"/>
+      <c r="Q50" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="R50" s="36"/>
+    </row>
+    <row r="51" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B51" s="36"/>
+      <c r="C51" s="35">
+        <f t="shared" si="6"/>
+        <v>0.20000000000000004</v>
+      </c>
+      <c r="D51" s="9">
+        <v>10</v>
+      </c>
+      <c r="E51" s="16">
+        <v>53</v>
+      </c>
+      <c r="F51" s="19">
+        <f t="shared" si="4"/>
+        <v>653</v>
+      </c>
+      <c r="G51" s="22">
+        <f>F51+H42</f>
+        <v>675</v>
+      </c>
+      <c r="H51" s="22"/>
+      <c r="I51" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="J51" s="36"/>
+      <c r="K51" s="35">
+        <f t="shared" si="7"/>
+        <v>0.20000000000000004</v>
+      </c>
+      <c r="L51" s="9">
+        <v>9</v>
+      </c>
+      <c r="M51" s="16">
+        <v>3</v>
+      </c>
+      <c r="N51" s="19">
+        <f t="shared" si="5"/>
+        <v>543</v>
+      </c>
+      <c r="O51" s="22">
+        <f>N51+P42</f>
+        <v>562</v>
+      </c>
+      <c r="P51" s="22"/>
+      <c r="Q51" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="R51" s="36"/>
+    </row>
+    <row r="52" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B52" s="36"/>
+      <c r="C52" s="35">
+        <f t="shared" si="6"/>
+        <v>0.10000000000000003</v>
+      </c>
+      <c r="D52" s="9">
+        <v>11</v>
+      </c>
+      <c r="E52" s="16">
+        <v>15</v>
+      </c>
+      <c r="F52" s="19">
+        <f t="shared" si="4"/>
+        <v>675</v>
+      </c>
+      <c r="G52" s="22">
+        <f>F52+H42</f>
+        <v>697</v>
+      </c>
+      <c r="H52" s="22"/>
+      <c r="I52" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="J52" s="36"/>
+      <c r="K52" s="35">
+        <f t="shared" si="7"/>
+        <v>0.10000000000000003</v>
+      </c>
+      <c r="L52" s="9">
+        <v>9</v>
+      </c>
+      <c r="M52" s="16">
+        <v>22</v>
+      </c>
+      <c r="N52" s="19">
+        <f t="shared" si="5"/>
+        <v>562</v>
+      </c>
+      <c r="O52" s="22">
+        <f>N52+P42</f>
+        <v>581</v>
+      </c>
+      <c r="P52" s="22"/>
+      <c r="Q52" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="R52" s="36"/>
+    </row>
+    <row r="53" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B53" s="36"/>
+      <c r="C53" s="40">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D53" s="41">
+        <v>11</v>
+      </c>
+      <c r="E53" s="42">
+        <v>37</v>
+      </c>
+      <c r="F53" s="43">
+        <f t="shared" si="4"/>
+        <v>697</v>
+      </c>
+      <c r="G53" s="44">
+        <f>F53+H42</f>
+        <v>719</v>
+      </c>
+      <c r="H53" s="44"/>
+      <c r="I53" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="J53" s="36"/>
+      <c r="K53" s="40">
+        <f>K52-0.1</f>
+        <v>0</v>
+      </c>
+      <c r="L53" s="41">
+        <v>9</v>
+      </c>
+      <c r="M53" s="42">
+        <v>41</v>
+      </c>
+      <c r="N53" s="43">
+        <f t="shared" si="5"/>
+        <v>581</v>
+      </c>
+      <c r="O53" s="44">
+        <f>N53+P42</f>
+        <v>600</v>
+      </c>
+      <c r="P53" s="44"/>
+      <c r="Q53" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="R53" s="36"/>
+    </row>
+    <row r="54" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B54" s="56"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="12"/>
+      <c r="J54" s="56"/>
+      <c r="K54" s="12"/>
+      <c r="L54" s="12"/>
+      <c r="M54" s="12"/>
+      <c r="N54" s="12"/>
+      <c r="O54" s="12"/>
+      <c r="P54" s="12"/>
+      <c r="Q54" s="12"/>
+      <c r="R54" s="56"/>
+    </row>
+    <row r="55" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="K55" s="1"/>
+    </row>
+    <row r="56" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="K56" s="1"/>
+    </row>
+    <row r="57" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="K57" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="19">
+    <mergeCell ref="O51:P51"/>
+    <mergeCell ref="O52:P52"/>
+    <mergeCell ref="O53:P53"/>
+    <mergeCell ref="O45:P45"/>
+    <mergeCell ref="O46:P46"/>
+    <mergeCell ref="O47:P47"/>
+    <mergeCell ref="O48:P48"/>
+    <mergeCell ref="O49:P49"/>
+    <mergeCell ref="O50:P50"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="G53:H53"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>